<commit_message>
Initial push: FAMS core features and setup
</commit_message>
<xml_diff>
--- a/data/users.xlsx
+++ b/data/users.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CE28ED-43C2-4444-B03A-4796E22D2986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Users" state="visible" r:id="rId4"/>
+    <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="36">
   <si>
     <t>username</t>
   </si>
@@ -26,19 +30,112 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Admin ID</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>HO</t>
+  </si>
+  <si>
+    <t>Kottayam</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>TamilNadu</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Manager1</t>
+  </si>
+  <si>
+    <t>Manager2</t>
+  </si>
+  <si>
+    <t>ManagerID</t>
+  </si>
+  <si>
+    <t>InitiateDisposalofAssets</t>
+  </si>
+  <si>
+    <t>InitiateTransfer</t>
+  </si>
+  <si>
+    <t>ApproveAssetCreation</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>AssetConfirmation</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ApproveDisposalofAssets</t>
+  </si>
+  <si>
+    <t>ApproveTransfer</t>
+  </si>
+  <si>
+    <t>GatePassCreation</t>
+  </si>
+  <si>
+    <t>Create/Modify Assets &amp; Initial Asset Mapping</t>
+  </si>
+  <si>
+    <t>InitiateAssetMappingtoBranchUsers</t>
+  </si>
+  <si>
+    <t>ApproveAssetMappingtoBranchUsers</t>
+  </si>
+  <si>
+    <t>BranchUser</t>
+  </si>
+  <si>
+    <t>ApproveBranchDetails</t>
+  </si>
+  <si>
+    <t>CreateBranchDetails</t>
+  </si>
+  <si>
+    <t>CreateAgreementInPayables</t>
+  </si>
+  <si>
+    <t>ApproveAgreementInPayables</t>
+  </si>
+  <si>
+    <t>CreateBillsInPayables</t>
+  </si>
+  <si>
+    <t>ApproveBillsInPayables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,12 +154,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,29 +522,505 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="A1:V7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.62890625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.68359375" style="3"/>
+    <col min="3" max="3" width="10.68359375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.1015625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" style="3"/>
+    <col min="6" max="6" width="9.734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.3125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="8.68359375" style="3"/>
+    <col min="15" max="15" width="9.5234375" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="8.68359375" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>123</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1">
+        <v>123463</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1">
+        <v>54321</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>